<commit_message>
Update userstories + Einde projectdag 1
</commit_message>
<xml_diff>
--- a/docs/userstories.xlsx
+++ b/docs/userstories.xlsx
@@ -11,14 +11,16 @@
     <sheet name="Personen" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Lucas">Personen!$A$1:$A$5</definedName>
     <definedName name="Personen">Personen!$A$1:$A$4</definedName>
+    <definedName name="Personen2">Personen!$A$1:$A$5</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Lucas</t>
   </si>
@@ -45,6 +47,30 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Slices</t>
+  </si>
+  <si>
+    <t>Webclient + ontwerp</t>
+  </si>
+  <si>
+    <t>C# Client</t>
+  </si>
+  <si>
+    <t>Unit testing</t>
+  </si>
+  <si>
+    <t>Overleggen + brainstormen</t>
+  </si>
+  <si>
+    <t>Iedereen</t>
+  </si>
+  <si>
+    <t>Programmeren aan hand van unit tests</t>
   </si>
 </sst>
 </file>
@@ -88,11 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,13 +426,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -430,41 +458,114 @@
       <c r="A2">
         <v>100</v>
       </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>300</v>
       </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>400</v>
       </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>600</v>
       </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>700</v>
       </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>800</v>
       </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -624,7 +725,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Geen geldige naam" sqref="D2:D40">
-      <formula1>Personen</formula1>
+      <formula1>Personen2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -634,10 +735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,6 +763,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Voorlopige invulling van userstory.
</commit_message>
<xml_diff>
--- a/docs/userstories.xlsx
+++ b/docs/userstories.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Lucas</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>Programmeren aan hand van unit tests</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Webclient coderen.</t>
+  </si>
+  <si>
+    <t>Box fixing en fixed nav + footer</t>
   </si>
 </sst>
 </file>
@@ -122,7 +134,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -138,9 +150,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +190,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -250,7 +262,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,16 +439,16 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.3984375" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -454,7 +466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>100</v>
       </c>
@@ -467,9 +479,14 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="2">
+        <v>42079</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>200</v>
       </c>
@@ -482,8 +499,14 @@
       <c r="D3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="2">
+        <v>42079</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>300</v>
       </c>
@@ -496,8 +519,14 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="2">
+        <v>42079</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>400</v>
       </c>
@@ -510,8 +539,14 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="2">
+        <v>42079</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>500</v>
       </c>
@@ -524,8 +559,14 @@
       <c r="D6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="2">
+        <v>42079</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>600</v>
       </c>
@@ -538,8 +579,14 @@
       <c r="D7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <v>42079</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>700</v>
       </c>
@@ -552,8 +599,14 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <v>42079</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>800</v>
       </c>
@@ -566,158 +619,194 @@
       <c r="D9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="2">
+        <v>42079</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>900</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>42080</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1000</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>42080</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1300</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1400</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1500</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1700</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1800</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1900</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>2100</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2200</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>2300</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2400</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>2500</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>2600</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>2700</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>2800</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>2900</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>3000</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>3100</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>3200</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>3300</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>3400</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>3500</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>3600</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>3700</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>3800</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>3900</v>
       </c>
@@ -741,29 +830,29 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Userstories 17/03 aanvullen & bug bij checkEmpySpots fixen
</commit_message>
<xml_diff>
--- a/docs/userstories.xlsx
+++ b/docs/userstories.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Lucas</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Datum</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Wireframes</t>
   </si>
   <si>
@@ -73,16 +70,19 @@
     <t>Programmeren aan hand van unit tests</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Finished</t>
-  </si>
-  <si>
     <t>Webclient coderen.</t>
   </si>
   <si>
     <t>Box fixing en fixed nav + footer</t>
+  </si>
+  <si>
+    <t>Algoritme voor diagonaal 4op een rij te vinden</t>
+  </si>
+  <si>
+    <t>Methodes voor UnitTest AI schrijven</t>
+  </si>
+  <si>
+    <t>UnitTests voor AI &amp; Diagonaal 4 op een rij te vinden</t>
   </si>
 </sst>
 </file>
@@ -134,7 +134,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -150,9 +150,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +190,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -262,7 +262,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,19 +436,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.3984375" customWidth="1"/>
-    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -462,16 +462,13 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -482,16 +479,13 @@
       <c r="E2" s="2">
         <v>42079</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -502,16 +496,13 @@
       <c r="E3" s="2">
         <v>42079</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>300</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -522,16 +513,13 @@
       <c r="E4" s="2">
         <v>42079</v>
       </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>400</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -542,16 +530,13 @@
       <c r="E5" s="2">
         <v>42079</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -562,16 +547,13 @@
       <c r="E6" s="2">
         <v>42079</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>600</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -582,36 +564,30 @@
       <c r="E7" s="2">
         <v>42079</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>700</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2">
         <v>42079</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>800</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -622,16 +598,13 @@
       <c r="E9" s="2">
         <v>42079</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>900</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -642,16 +615,13 @@
       <c r="E10" s="2">
         <v>42080</v>
       </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1000</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -662,151 +632,184 @@
       <c r="E11" s="2">
         <v>42080</v>
       </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1100</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>42080</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1200</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>42080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1300</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>42080</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1400</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1500</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1600</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1700</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1800</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1900</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2100</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2200</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2300</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2400</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2500</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2600</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2700</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2800</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2900</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3000</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3100</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3200</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3300</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3400</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3500</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3600</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3700</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3800</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3900</v>
       </c>
@@ -830,31 +833,31 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>